<commit_message>
Write Data from Excel to DB
</commit_message>
<xml_diff>
--- a/Load_FromDB.xlsx
+++ b/Load_FromDB.xlsx
@@ -140,107 +140,107 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" t="n" s="0">
+      <c r="B3" t="n" s="0">
         <v>25.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="C4" t="n" s="0">
+      <c r="B4" t="n" s="0">
         <v>30.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="C5" t="n" s="0">
+      <c r="B5" t="n" s="0">
         <v>22.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="C6" t="n" s="0">
+      <c r="B6" t="n" s="0">
         <v>28.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="C7" t="n" s="0">
+      <c r="B7" t="n" s="0">
         <v>35.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="C8" t="n" s="0">
+      <c r="B8" t="n" s="0">
         <v>29.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="C9" t="n" s="0">
+      <c r="B9" t="n" s="0">
         <v>31.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="C10" t="n" s="0">
+      <c r="B10" t="n" s="0">
         <v>26.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="C11" t="n" s="0">
+      <c r="B11" t="n" s="0">
         <v>27.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="C12" t="n" s="0">
+      <c r="B12" t="n" s="0">
         <v>24.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="C13" t="n" s="0">
+      <c r="B13" t="n" s="0">
         <v>33.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="C14" t="n" s="0">
+      <c r="B14" t="n" s="0">
         <v>32.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="C15" t="n" s="0">
+      <c r="B15" t="n" s="0">
         <v>28.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="C16" t="n" s="0">
+      <c r="B16" t="n" s="0">
         <v>23.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="C17" t="n" s="0">
+      <c r="B17" t="n" s="0">
         <v>34.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="C18" t="n" s="0">
+      <c r="B18" t="n" s="0">
         <v>25.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="C19" t="n" s="0">
+      <c r="B19" t="n" s="0">
         <v>29.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20" t="n" s="0">
+      <c r="B20" t="n" s="0">
         <v>21.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="C21" t="n" s="0">
+      <c r="B21" t="n" s="0">
         <v>36.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="C22" t="n" s="0">
+      <c r="B22" t="n" s="0">
         <v>27.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="C23" t="n" s="0">
+      <c r="B23" t="n" s="0">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>